<commit_message>
Add tests to cover fixed functionality
</commit_message>
<xml_diff>
--- a/tests/framework_junction_timed_remainder_test.xlsx
+++ b/tests/framework_junction_timed_remainder_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romesh\projects\atomica\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41DC712-0172-4E68-88B6-7D2EE1526B2B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EAE908-A9B9-444B-A859-EE719DF70D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4455" yWindow="2940" windowWidth="32880" windowHeight="15150" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5370" yWindow="3120" windowWidth="31800" windowHeight="15195" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Databook Pages" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -570,7 +575,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="48">
   <si>
     <t>Datasheet Code Name</t>
   </si>
@@ -653,28 +658,16 @@
     <t>proportion</t>
   </si>
   <si>
-    <t>s1</t>
-  </si>
-  <si>
-    <t>s2</t>
-  </si>
-  <si>
     <t>j1</t>
   </si>
   <si>
     <t>j2</t>
   </si>
   <si>
-    <t>Sink 1</t>
-  </si>
-  <si>
     <t>Junction 2</t>
   </si>
   <si>
     <t>Junction 1</t>
-  </si>
-  <si>
-    <t>Sink 2</t>
   </si>
   <si>
     <t>p1</t>
@@ -686,16 +679,46 @@
     <t>&gt;</t>
   </si>
   <si>
-    <t>p2</t>
+    <t>c1</t>
   </si>
   <si>
-    <t>Proportion to S2</t>
+    <t>Compartment 1</t>
   </si>
   <si>
-    <t>s3</t>
+    <t>j3</t>
   </si>
   <si>
-    <t>Sink 3</t>
+    <t>Junction 3</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>Compartment 2</t>
+  </si>
+  <si>
+    <t>c3</t>
+  </si>
+  <si>
+    <t>Compartment 3</t>
+  </si>
+  <si>
+    <t>state_dur</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>Timed</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>Continue</t>
   </si>
 </sst>
 </file>
@@ -738,12 +761,15 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp"/>
     </fill>
   </fills>
   <borders count="1">
@@ -758,7 +784,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -779,11 +805,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="19">
     <dxf>
       <fill>
         <patternFill>
@@ -864,20 +892,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -914,104 +928,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1404,7 +1320,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="19" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1417,10 +1333,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,21 +1405,18 @@
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>29</v>
+      <c r="A3" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="2" t="s">
+      <c r="I3" t="s">
         <v>16</v>
       </c>
       <c r="K3" s="2"/>
@@ -1514,9 +1427,9 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="2"/>
@@ -1526,14 +1439,14 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="2"/>
@@ -1544,76 +1457,77 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>30</v>
+      <c r="A6" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>41</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="B1:B2 B7:B1048576">
-    <cfRule type="expression" dxfId="18" priority="7">
+  <conditionalFormatting sqref="B1:B3 B6:B1048576">
+    <cfRule type="expression" dxfId="17" priority="7">
       <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:I1048576">
-    <cfRule type="expression" dxfId="17" priority="5">
-      <formula>AND(J4&lt;&gt;"",NOT(I4&lt;&gt;""))</formula>
+  <conditionalFormatting sqref="I5:I1048576">
+    <cfRule type="expression" dxfId="16" priority="5">
+      <formula>AND(J5&lt;&gt;"",NOT(I5&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I5">
-    <cfRule type="expression" dxfId="16" priority="11">
-      <formula>AND(J2&lt;&gt;"",NOT(I3&lt;&gt;""))</formula>
+  <conditionalFormatting sqref="A4:A5">
+    <cfRule type="expression" dxfId="15" priority="12">
+      <formula>AND(#REF!&lt;&gt;"",NOT(A4&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A6">
-    <cfRule type="expression" dxfId="15" priority="12">
-      <formula>AND(#REF!&lt;&gt;"",NOT(A3&lt;&gt;""))</formula>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="expression" dxfId="14" priority="2">
+      <formula>AND(#REF!&lt;&gt;"",NOT(B5&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:B6">
-    <cfRule type="expression" dxfId="14" priority="2">
+  <conditionalFormatting sqref="B4">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>AND(#REF!&lt;&gt;"",NOT(B4&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="12" priority="1">
-      <formula>AND(#REF!&lt;&gt;"",NOT(B3&lt;&gt;""))</formula>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="expression" dxfId="12" priority="17">
+      <formula>AND(J2&lt;&gt;"",NOT(I4&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
-    <cfRule type="expression" dxfId="11" priority="17">
-      <formula>AND(J4&lt;&gt;"",NOT(I6&lt;&gt;""))</formula>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="expression" dxfId="10" priority="25">
+      <formula>AND(#REF!&lt;&gt;"",NOT(I5&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576 C1:E1048576" xr:uid="{EFA3D3D9-56A8-43F0-A737-1EDBC3038312}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:E1048576 H1:H1048576" xr:uid="{EFA3D3D9-56A8-43F0-A737-1EDBC3038312}">
       <formula1>"n,y"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1625,7 +1539,7 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="4" id="{0238372B-F012-4B98-A58B-305EDC0BD903}">
-            <xm:f>AND(I3&lt;&gt;"",ISERROR(MATCH(I3,'Databook Pages'!$A:$A,0)))</xm:f>
+            <xm:f>AND(I4&lt;&gt;"",ISERROR(MATCH(I4,'Databook Pages'!$A:$A,0)))</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -1634,7 +1548,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I1048576</xm:sqref>
+          <xm:sqref>I4:I1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1644,7 +1558,7 @@
           <x14:formula1>
             <xm:f>'Databook Pages'!$A$2:$A$9999</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I1048576</xm:sqref>
+          <xm:sqref>I4:I1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1657,10 +1571,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:OH396"/>
+  <dimension ref="A1:OG395"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1668,12 +1582,12 @@
     <col min="1" max="1" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:398" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:397" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
-        <v>29</v>
+      <c r="B1" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="C1" t="s">
         <v>27</v>
@@ -1681,13 +1595,20 @@
       <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
-        <v>30</v>
+      <c r="E1" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="L1" s="3" t="str">
+        <f>IF(Compartments!$A13&lt;&gt;"",Compartments!$A13,"")</f>
+        <v/>
+      </c>
       <c r="M1" s="3" t="str">
         <f>IF(Compartments!$A14&lt;&gt;"",Compartments!$A14,"")</f>
         <v/>
@@ -3228,12 +3149,8 @@
         <f>IF(Compartments!$A398&lt;&gt;"",Compartments!$A398,"")</f>
         <v/>
       </c>
-      <c r="OH1" s="3" t="str">
-        <f>IF(Compartments!$A399&lt;&gt;"",Compartments!$A399,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="2" spans="1:398" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:397" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -3241,59 +3158,94 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:398" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
+    <row r="3" spans="1:397" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="9"/>
       <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:397" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:397" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:397" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:397" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:398" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:398" x14ac:dyDescent="0.25">
+      <c r="F7" s="9"/>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:397" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="str">
+        <f>IF(Compartments!$A13&lt;&gt;"",Compartments!$A13,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:397" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="str">
         <f>IF(Compartments!$A14&lt;&gt;"",Compartments!$A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:398" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:397" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="str">
         <f>IF(Compartments!$A15&lt;&gt;"",Compartments!$A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:398" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:397" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="str">
         <f>IF(Compartments!$A16&lt;&gt;"",Compartments!$A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:398" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:397" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="str">
         <f>IF(Compartments!$A17&lt;&gt;"",Compartments!$A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:398" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:397" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="str">
         <f>IF(Compartments!$A18&lt;&gt;"",Compartments!$A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:398" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:397" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="str">
         <f>IF(Compartments!$A19&lt;&gt;"",Compartments!$A19,"")</f>
         <v/>
@@ -5573,36 +5525,25 @@
         <v/>
       </c>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A396" s="3" t="str">
-        <f>IF(Compartments!$A399&lt;&gt;"",Compartments!$A399,"")</f>
-        <v/>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:A8">
-    <cfRule type="expression" dxfId="10" priority="4">
-      <formula>AND(#REF!&lt;&gt;"",NOT(A5&lt;&gt;""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:J1">
-    <cfRule type="expression" dxfId="9" priority="3">
+  <conditionalFormatting sqref="G1:I1">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>AND(#REF!&lt;&gt;"",NOT(G1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A4">
+  <conditionalFormatting sqref="A4:A5">
     <cfRule type="expression" dxfId="7" priority="2">
-      <formula>AND(#REF!&lt;&gt;"",NOT(A3&lt;&gt;""))</formula>
+      <formula>AND(#REF!&lt;&gt;"",NOT(A4&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:E1">
+  <conditionalFormatting sqref="C1:D1">
     <cfRule type="expression" dxfId="6" priority="1">
-      <formula>AND(#REF!&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
+      <formula>AND(#REF!&lt;&gt;"",NOT(C1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Code names must be unique" error="Parameter code names must be unique" sqref="B2" xr:uid="{6909806C-167F-4746-8AD1-D1EA1D2F8258}">
-      <formula1>COUNTIF(B:B,B2)&lt;2</formula1>
+      <formula1>COUNTIF(#REF!,B2)&lt;2</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5612,7 +5553,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="6" id="{51D293C8-E19A-4195-82DA-432679B2823C}">
+          <x14:cfRule type="expression" priority="8" id="{51D293C8-E19A-4195-82DA-432679B2823C}">
             <xm:f>AND(AND(B2&lt;&gt;"&gt;",B2&lt;&gt;""),ISERROR(MATCH(B2,Parameters!$A:$A,0)))</xm:f>
             <x14:dxf>
               <fill>
@@ -5622,7 +5563,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C2:XFD2 B3:XFD1048576</xm:sqref>
+          <xm:sqref>B2:XFD1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -5750,10 +5691,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5765,7 +5706,7 @@
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5781,8 +5722,11 @@
       <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -5799,56 +5743,73 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
+        <v>47</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="D3" s="7">
-        <v>0.6</v>
+        <v>200</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="7">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="7">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E10" s="2"/>
     </row>
   </sheetData>
@@ -5868,7 +5829,8 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>

</xml_diff>